<commit_message>
Update table svg's for number formats that changed
</commit_message>
<xml_diff>
--- a/resources/dataframes_THS_9th_removed.xlsx
+++ b/resources/dataframes_THS_9th_removed.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="145">
   <si>
     <t>Student ID</t>
   </si>
@@ -458,69 +458,6 @@
   </si>
   <si>
     <t>84.6</t>
-  </si>
-  <si>
-    <t>78.5</t>
-  </si>
-  <si>
-    <t>81.6</t>
-  </si>
-  <si>
-    <t>93.5</t>
-  </si>
-  <si>
-    <t>87.1</t>
-  </si>
-  <si>
-    <t>73.5</t>
-  </si>
-  <si>
-    <t>66.2</t>
-  </si>
-  <si>
-    <t>96.6</t>
-  </si>
-  <si>
-    <t>92.7</t>
-  </si>
-  <si>
-    <t>81.1</t>
-  </si>
-  <si>
-    <t>90.4</t>
-  </si>
-  <si>
-    <t>62.8</t>
-  </si>
-  <si>
-    <t>53.5</t>
-  </si>
-  <si>
-    <t>93.6</t>
-  </si>
-  <si>
-    <t>70.0</t>
-  </si>
-  <si>
-    <t>96.1</t>
-  </si>
-  <si>
-    <t>96.7</t>
-  </si>
-  <si>
-    <t>89.9</t>
-  </si>
-  <si>
-    <t>90.6</t>
-  </si>
-  <si>
-    <t>58.3</t>
-  </si>
-  <si>
-    <t>66.5</t>
-  </si>
-  <si>
-    <t>53.7</t>
   </si>
 </sst>
 </file>
@@ -1204,40 +1141,40 @@
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" t="s">
-        <v>154</v>
+      <c r="B2">
+        <v>83.4654254168185</v>
+      </c>
+      <c r="C2">
+        <v>83.9023147557395</v>
+      </c>
+      <c r="D2">
+        <v>93.61001987197841</v>
+      </c>
+      <c r="E2">
+        <v>96.55022312941765</v>
+      </c>
+      <c r="F2">
+        <v>90.39253262434622</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" t="s">
-        <v>165</v>
+      <c r="B3">
+        <v>76.95673306832398</v>
+      </c>
+      <c r="C3">
+        <v>80.96663632734915</v>
+      </c>
+      <c r="D3">
+        <v>66.54845257144746</v>
+      </c>
+      <c r="E3">
+        <v>80.79906211395057</v>
+      </c>
+      <c r="F3">
+        <v>53.67220822778149</v>
       </c>
     </row>
   </sheetData>
@@ -2931,80 +2868,80 @@
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" t="s">
-        <v>154</v>
+      <c r="B2">
+        <v>83.45539900855027</v>
+      </c>
+      <c r="C2">
+        <v>83.93381405396646</v>
+      </c>
+      <c r="D2">
+        <v>93.46009572653237</v>
+      </c>
+      <c r="E2">
+        <v>96.61087677671375</v>
+      </c>
+      <c r="F2">
+        <v>90.36945874402643</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" t="s">
-        <v>136</v>
+      <c r="B3">
+        <v>81.8998257021498</v>
+      </c>
+      <c r="C3">
+        <v>83.15528577020937</v>
+      </c>
+      <c r="D3">
+        <v>87.13353760737169</v>
+      </c>
+      <c r="E3">
+        <v>92.71820457965273</v>
+      </c>
+      <c r="F3">
+        <v>81.41859632428398</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" t="s">
-        <v>155</v>
+      <c r="B4">
+        <v>78.50200163320186</v>
+      </c>
+      <c r="C4">
+        <v>81.63626134231335</v>
+      </c>
+      <c r="D4">
+        <v>73.46258857734237</v>
+      </c>
+      <c r="E4">
+        <v>84.3192605609222</v>
+      </c>
+      <c r="F4">
+        <v>62.7782334137728</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" t="s">
-        <v>156</v>
+      <c r="B5">
+        <v>76.99720981240274</v>
+      </c>
+      <c r="C5">
+        <v>81.02784255713441</v>
+      </c>
+      <c r="D5">
+        <v>66.16481311032456</v>
+      </c>
+      <c r="E5">
+        <v>81.13395072128019</v>
+      </c>
+      <c r="F5">
+        <v>53.5268548869691</v>
       </c>
     </row>
   </sheetData>
@@ -3044,60 +2981,60 @@
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F2" t="s">
-        <v>161</v>
+      <c r="B2">
+        <v>83.82159776422071</v>
+      </c>
+      <c r="C2">
+        <v>83.92984341754834</v>
+      </c>
+      <c r="D2">
+        <v>93.55022469776569</v>
+      </c>
+      <c r="E2">
+        <v>96.09943667320715</v>
+      </c>
+      <c r="F2">
+        <v>89.88385340844357</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F3" t="s">
-        <v>162</v>
+      <c r="B3">
+        <v>83.36120143857568</v>
+      </c>
+      <c r="C3">
+        <v>83.87386873887871</v>
+      </c>
+      <c r="D3">
+        <v>93.58239833305436</v>
+      </c>
+      <c r="E3">
+        <v>96.7326541730898</v>
+      </c>
+      <c r="F3">
+        <v>90.55799747596197</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" t="s">
-        <v>163</v>
+      <c r="B4">
+        <v>77.746416511437</v>
+      </c>
+      <c r="C4">
+        <v>81.34449272598371</v>
+      </c>
+      <c r="D4">
+        <v>69.96336073939453</v>
+      </c>
+      <c r="E4">
+        <v>82.7666344526415</v>
+      </c>
+      <c r="F4">
+        <v>58.28600304906789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>